<commit_message>
pushing nin code changes
</commit_message>
<xml_diff>
--- a/data/scraped_index.xlsx
+++ b/data/scraped_index.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,211 +452,211 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20724502537</v>
+        <v>300724004056</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-senior-manager-data-science-and-analytics-metafolks-pune-5-to-10-years-020724502537</t>
+          <t>https://www.naukri.com/job-listings-data-analyst-data-science-sr-trainer-talentify-hyderabad-pune-bengaluru-6-to-11-years-300724004056</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Senior Manager - Data Science and Analytics_20724502537.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Analyst- Data Science  Sr Trainer_300724004056.xlsx</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>30724001182</v>
+        <v>290724500690</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-data-analytics-data-science-trainers-prowess-publishing-hyderabad-pune-4-to-9-years-030724001182</t>
+          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-9-years-290724500690</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Analytics-Data Science Trainers_30724001182.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_290724500690.xlsx</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20724010574</v>
+        <v>290724500689</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-data-science-manager-axa-global-business-services-pune-bengaluru-8-to-13-years-020724010574</t>
+          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-9-years-290724500689</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Manager_20724010574.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_290724500689.xlsx</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>240524012199</v>
+        <v>140324012002</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-hiring-data-science-engineer-lead-architect-xoriant-hyderabad-pune-mumbai-all-areas-5-to-10-years-240524012199</t>
+          <t>https://www.naukri.com/job-listings-data-science-manager-axtria-pune-gurugram-bengaluru-8-to-12-years-140324012002</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Hiring Data Science Engineer - Lead - Architect !_240524012199.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Manager_140324012002.xlsx</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>280524500123</v>
+        <v>170724900002</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-9-years-280524500123</t>
+          <t>https://www.naukri.com/job-listings-s-c-global-network-ai-cg-s-consultant-data-science-accenture-solutions-pvt-ltd-pune-5-to-10-years-170724900002</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_280524500123.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/S&amp;C Global Network - AI - CG&amp;S - Consultant Data Science_170724900002.xlsx</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>310524005756</v>
+        <v>240524012199</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-lead-data-science-nitor-pune-6-to-9-years-310524005756</t>
+          <t>https://www.naukri.com/job-listings-hiring-data-science-engineer-lead-architect-xoriant-hyderabad-pune-mumbai-all-areas-5-to-10-years-240524012199</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Lead Data Science_310524005756.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Hiring Data Science Engineer - Lead - Architect !_240524012199.xlsx</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>70323501288</v>
+        <v>240724909755</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-senior-analyst-data-science-navit-software-solutions-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-8-years-070323501288</t>
+          <t>https://www.naukri.com/job-listings-data-science-manager-4bell-technology-mumbai-indore-pune-8-to-13-years-240724909755</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Senior Analyst Data Science_70323501288.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Manager_240724909755.xlsx</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>240424500189</v>
+        <v>160724500785</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-consultant-data-science-analytics-transunion-software-services-pvt-ltd-pune-chennai-4-to-8-years-240424500189</t>
+          <t>https://www.naukri.com/job-listings-manager-data-science-genai-tmt-vertical-trendence-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-4-to-8-years-160724500785</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Consultant - Data Science &amp; Analytics_240424500189.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Manager - Data Science (GenAI) - TMT Vertical_160724500785.xlsx</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>160524502594</v>
+        <v>20724502537</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-2-to-8-years-160524502594</t>
+          <t>https://www.naukri.com/job-listings-senior-manager-data-science-and-analytics-metafolks-pune-5-to-10-years-020724502537</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_160524502594.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Senior Manager - Data Science and Analytics_20724502537.xlsx</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>160524502269</v>
+        <v>70323501288</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-7-to-10-years-160524502269</t>
+          <t>https://www.naukri.com/job-listings-senior-analyst-data-science-navit-software-solutions-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-8-years-070323501288</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_160524502269.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Senior Analyst Data Science_70323501288.xlsx</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>160524502177</v>
+        <v>120724004528</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-6-to-9-years-160524502177</t>
+          <t>https://www.naukri.com/job-listings-data-science-engineer-gen-ai-is-required-perm-role-ibm-pune-chennai-bengaluru-5-to-10-years-120724004528</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_160524502177.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Engineer- GEN AI is required-PERM ROLE_120724004528.xlsx</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>50424500273</v>
+        <v>20724010574</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-aws-data-science-platform-engineer-cosmic-it-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-7-to-12-years-050424500273</t>
+          <t>https://www.naukri.com/job-listings-data-science-manager-axa-global-business-services-pune-bengaluru-8-to-13-years-020724010574</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/AWS Data Science Platform Engineer_50424500273.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Manager_20724010574.xlsx</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>261023501559</v>
+        <v>50724905401</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-data-science-engineer-cognisure-pune-bengaluru-7-to-10-years-261023501559</t>
+          <t>https://www.naukri.com/job-listings-data-science-practitioner-accenture-solutions-pvt-ltd-pune-5-to-10-years-050724905401</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Engineer_261023501559.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Practitioner_50724905401.xlsx</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>50624013599</v>
+        <v>261023501559</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-data-science-engineer-chase-hr-consulting-hyderabad-pune-bengaluru-4-to-9-years-050624013599</t>
+          <t>https://www.naukri.com/job-listings-data-science-engineer-cognisure-pune-bengaluru-7-to-10-years-261023501559</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Engineer_50624013599.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Engineer_261023501559.xlsx</t>
         </is>
       </c>
     </row>
@@ -677,76 +677,271 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>20424500275</v>
+        <v>40624501335</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-consultant-data-science-analytics-transunion-software-services-pvt-ltd-pune-4-to-8-years-020424500275</t>
+          <t>https://www.naukri.com/job-listings-data-science-nextcomm-corporation-india-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-1-to-8-years-040624501335</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Consultant - Data Science &amp; Analytics_20424500275.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science_40624501335.xlsx</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>130524003568</v>
+        <v>30724010023</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-hexaware-looking-immediate-joiners-senior-data-scientist-nlp-genai-hexaware-technologies-navi-mumbai-pune-chennai-5-to-9-years-130524003568</t>
+          <t>https://www.naukri.com/job-listings-faculty-data-science-analytics-prowess-publishing-hyderabad-pune-3-to-8-years-030724010023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Hexaware_ Looking Immediate joiners Senior Data Scientist NLP-GenAI_130524003568.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Faculty - Data Science &amp; Analytics_30724010023.xlsx</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>40624501335</v>
+        <v>290724502209</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-data-science-nextcomm-corporation-india-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-1-to-8-years-040624501335</t>
+          <t>https://www.naukri.com/job-listings-data-scientist-agilite-global-solutions-company-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-10-years-290724502209</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science_40624501335.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Scientist_290724502209.xlsx</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>30724010023</v>
+        <v>290724501408</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-faculty-data-science-analytics-prowess-publishing-hyderabad-pune-3-to-8-years-030724010023</t>
+          <t>https://www.naukri.com/job-listings-data-scientist-norstella-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-10-years-290724501408</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Faculty - Data Science &amp; Analytics_30724010023.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Scientist_290724501408.xlsx</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>240624006543</v>
+        <v>230724013592</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.naukri.com/job-listings-data-scientist-mantra-technologies-kolkata-hyderabad-pune-ahmedabad-chennai-bengaluru-delhi-ncr-mumbai-all-areas-4-to-8-years-240624006543</t>
+          <t>https://www.naukri.com/job-listings-senior-data-scientist-nvidia-intel-ai-ltimindtree-pune-chennai-bengaluru-5-to-10-years-230724013592</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Scientist_240624006543.xlsx</t>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Senior Data Scientist - Nvidia Intel AI_230724013592.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>60924012222</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-data-science-consultant-optimization-supply-chain-and-manufacturing-zs-pune-bengaluru-6-to-9-years-060924012222</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Consultant (Optimization - Supply Chain and Manufacturing_60924012222.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>280824916175</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-data-science-engineer-cybage-software-pvt-ltd-pune-8-to-12-years-280824916175</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Engineer_280824916175.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>260824913880</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-data-science-professional-capgemini-technology-services-india-limited-hyderabad-pune-bengaluru-6-to-9-years-260824913880</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/DATA SCIENCE Professional_260824913880.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>210824500836</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-6-to-9-years-210824500836</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_210824500836.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>10824501631</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-analytics-data-science-and-iot-lead-hexaware-technologies-ltd-kolkata-mumbai-new-delhi-hyderabad-pune-chennai-bengaluru-5-to-9-years-010824501631</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Analytics Data science and IOT Lead_10824501631.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>80824500328</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-senior-platform-automation-data-science-engineer-mastercard-pune-4-to-8-years-080824500328</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Senior Platform Automation &amp; Data Science Engineer_80824500328.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>220824503831</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-lead-data-science-engineer-wolters-kluwer-medknow-publications-pune-5-to-10-years-220824503831</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Lead Data Science Engineer_220824503831.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>230824502289</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-manager-data-science-tredence-kolkata-pune-chennai-gurugram-bengaluru-8-to-13-years-230824502289</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Manager - Data Science_230824502289.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>250824000014</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-data-science-engineer-r-studio-integrated-personnel-services-pune-chennai-bengaluru-4-to-8-years-250824000014</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Engineer (R Studio)_250824000014.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>140824913740</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-lead-data-science-nitor-infotech-pvt-ltd-pune-6-to-9-years-140824913740</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Lead Data Science_140824913740.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>100824005069</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-lead-data-science-nitor-pune-6-to-9-years-100824005069</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Lead Data Science_100824005069.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>281022502443</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-data-science-professional-extentia-information-technology-pune-4-to-9-years-281022502443</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Science Professional_281022502443.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>271122001064</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.naukri.com/job-listings-data-scientist-consultant-aarons-visions-hyderabad-pune-bengaluru-6-to-11-years-271122001064</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>/home/ravindra/git_repos/monitoring_ds_jobs/data/scraped_data/Data Scientist Consultant_271122001064.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>